<commit_message>
fix: cope with troubles in 17th, 26th (two ways), 5th tasks
9th task left
</commit_message>
<xml_diff>
--- a/Bariants/fipi-04-29/Задание 9/9.xlsx
+++ b/Bariants/fipi-04-29/Задание 9/9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htmlprogrammist/Python/ege/Bariants/fipi-04-29/Задание 9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7CA031-C258-6E4C-AC51-82A837C1157A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11815E5-2ACE-374A-AB81-04DC83BB2811}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>MID</t>
+  </si>
+  <si>
+    <t>правильный ответ: 5</t>
   </si>
 </sst>
 </file>
@@ -154,7 +157,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -206,7 +209,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -411,8 +414,8 @@
   <dimension ref="A1:AB105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AC11" sqref="AC11"/>
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -654,8 +657,8 @@
         <v>15.3</v>
       </c>
       <c r="AA3" s="4">
-        <f>MAX(B2:Y2,B62:Y62)</f>
-        <v>29.3</v>
+        <f>MAX(K2:N62)</f>
+        <v>28.8</v>
       </c>
       <c r="AB3" s="4">
         <f>AVERAGE(B2:Y62)</f>
@@ -817,7 +820,7 @@
       </c>
       <c r="AA5" s="4">
         <f>AA3-AB3</f>
-        <v>8.6794398907103947</v>
+        <v>8.1794398907103947</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
@@ -898,6 +901,9 @@
       </c>
       <c r="AA6" s="6">
         <v>8</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: added a solution for the second part of the approbation
</commit_message>
<xml_diff>
--- a/Bariants/fipi-04-29/Задание 9/9.xlsx
+++ b/Bariants/fipi-04-29/Задание 9/9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htmlprogrammist/Python/ege/Bariants/fipi-04-29/Задание 9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11815E5-2ACE-374A-AB81-04DC83BB2811}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDBFFA4-4C0C-E24B-9210-910FD7EBD447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,7 +415,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA10" sqref="AA10"/>
+      <selection pane="topRight" activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -661,8 +661,8 @@
         <v>28.8</v>
       </c>
       <c r="AB3" s="4">
-        <f>AVERAGE(B2:Y62)</f>
-        <v>20.620560109289606</v>
+        <f>AVERAGE(K2:N62)</f>
+        <v>23.098360655737697</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
@@ -820,7 +820,7 @@
       </c>
       <c r="AA5" s="4">
         <f>AA3-AB3</f>
-        <v>8.1794398907103947</v>
+        <v>5.7016393442623041</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
@@ -900,7 +900,7 @@
         <v>14.7</v>
       </c>
       <c r="AA6" s="6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AB6" t="s">
         <v>3</v>

</xml_diff>